<commit_message>
Add part b and backend of the procces
</commit_message>
<xml_diff>
--- a/Parte A/Data/data_train_cleaned.xlsx
+++ b/Parte A/Data/data_train_cleaned.xlsx
@@ -458,7 +458,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>hi really know phrase situation try life really good point right never really depressed stuff percent time mind clear graduate high school really excite however people family friend group ton issue wether sleep day hate ambition keep living world get problem want sound like gloat usually person lot people end go usually able talk people issue help long run yeah sometimes issue make really sad stuff feel sad people tell feel worthless today best friend show cut really effect talk mostly painfully bore even know pretty logical guy go class sit hour time nothing challenge way school work clinically diagnose depression psychiatric ward see therapist regularly couple hour since show arm even see get main problem right first really know help say literally thing really hang school weekend sit bed day try make effort much need say long go highschool consider law go feel way graduate need know something help tell parent therapist help already go talk tomorrow know second stuff like really effect feel world unfair everyone care want everyone love feel well lately feel depress whenever friend need talk issue really weigh want leave people care dirt yeah anyone advice whatsoever please help normally able deal feeling help friend right struggle thank red_heart</t>
+          <t>hi really know phrase situation try life really good point right never really depressed stuff percent time mind clear graduate high school really excite however people family friend group ton issue wether sleep day hate ambition keep living world get problem want sound like gloat usually person lot people end go usually able talk people issue help long run yeah sometimes issue make really sad stuff feel sad people tell feel worthless today best friend show cut really effect talk mostly painfully bore even know pretty logical guy go class sit hour time nothing challenge way school work clinically diagnose depression psychiatric ward see therapist regularly couple hour since show arm even see get main problem right first really know help say literally thing really hang school weekend sit bed day try make effort much need say long go highschool consider law go feel way graduate need know something help tell parent therapist help already go talk tomorrow know second stuff like really effect feel world unfair everyone care want everyone love feel well lately feel depress whenever friend need talk issue really weigh want leave people care dirt yeah anyone advice whatsoever please help normally able deal feeling help friend right struggle thank</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2022,7 +2022,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>another thing mom recommend consider grief therapy group normal therapy group think still grieve might process group many time sometimes felt okay others idea deal far cripple depression time bad home life bpd point either man_facepalming therapist seem like really know help like maybe personality case level actually consider get back group know maybe time actually help try closed get bad start shift personality interact mom anyone call hope make sense hope guy comfortable day send good vibe way</t>
+          <t>another thing mom recommend consider grief therapy group normal therapy group think still grieve might process group many time sometimes felt okay others idea deal far cripple depression time bad home life bpd point either therapist seem like really know help like maybe personality case level actually consider get back group know maybe time actually help try closed get bad start shift personality interact mom anyone call hope make sense hope guy comfortable day send good vibe way</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2243,7 +2243,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>title say full upper body workout cope thought head blast pilot sign_of_the_horns today pretty shit day bad hair entire day shit get home voice return kept tell piece shit get question learn love</t>
+          <t>title say full upper body workout cope thought head blast pilot today pretty shit day bad hair entire day shit get home voice return kept tell piece shit get question learn love</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -4721,7 +4721,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>nice know finally come home mara tara red_heart</t>
+          <t>nice know finally come home mara tara</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
@@ -4891,7 +4891,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>break toxic boyfriend today come cry back tell give u break love much can not keep take shit keep tell thing get good change never know hard take back please someone help give inloudly_crying_face</t>
+          <t>break toxic boyfriend today come cry back tell give u break love much can not keep take shit keep tell thing get good change never know hard take back please someone help give</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
@@ -6523,7 +6523,7 @@
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>real life friend sometimes talk people school mutual subject never get call school weekend decent grade live comfortably like try approachable try nice always shut ask go away want go therapist friday tire living constant state loneliness isolation begin slit area arm shoulder elbow want people see know pain everyday go school smile face come home cry like nothing worthless know hop accomplish say hey story confused_face</t>
+          <t>real life friend sometimes talk people school mutual subject never get call school weekend decent grade live comfortably like try approachable try nice always shut ask go away want go therapist friday tire living constant state loneliness isolation begin slit area arm shoulder elbow want people see know pain everyday go school smile face come home cry like nothing worthless know hop accomplish say hey story</t>
         </is>
       </c>
       <c r="C359" t="inlineStr">
@@ -6608,7 +6608,7 @@
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>pretty much deal depression anxiety quite number year go real low rough patch moment self hatred grow rapidly top ex girlfriend break day wondering could comment positive thing like inspiration whatnot thank advance hope everyone read right cop alright never alone red_heart</t>
+          <t>pretty much deal depression anxiety quite number year go real low rough patch moment self hatred grow rapidly top ex girlfriend break day wondering could comment positive thing like inspiration whatnot thank advance hope everyone read right cop alright never alone</t>
         </is>
       </c>
       <c r="C364" t="inlineStr">
@@ -8444,7 +8444,7 @@
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>hey question anyone willing answer would like know anyone cut past maybe still cut help way relive sort distress know dangerous game play curious cheer everyone hope stay life continue least try conquer demon might think love love someone might want someone ask ok milk end sort progression get good please stay life struggle want push forward see anything get good feel free answer question would like love night everyone red_heart</t>
+          <t>hey question anyone willing answer would like know anyone cut past maybe still cut help way relive sort distress know dangerous game play curious cheer everyone hope stay life continue least try conquer demon might think love love someone might want someone ask ok milk end sort progression get good please stay life struggle want push forward see anything get good feel free answer question would like love night everyone</t>
         </is>
       </c>
       <c r="C472" t="inlineStr">
@@ -11789,7 +11789,7 @@
       </c>
       <c r="B669" t="inlineStr">
         <is>
-          <t>reason alive fact want people care feel pain suffer go everyday commit suicide loudly_crying_face want live anymore</t>
+          <t>reason alive fact want people care feel pain suffer go everyday commit suicide want live anymore</t>
         </is>
       </c>
       <c r="C669" t="inlineStr">
@@ -12766,7 +12766,7 @@
     <row r="727">
       <c r="A727" t="inlineStr">
         <is>
-          <t>personal crisis go write internet hey welcome ted talk waving_hand_mediumlight_skin_tone</t>
+          <t>personal crisis go write internet hey welcome ted talk</t>
         </is>
       </c>
       <c r="B727" t="inlineStr">
@@ -13294,7 +13294,7 @@
       </c>
       <c r="B758" t="inlineStr">
         <is>
-          <t>change diet help within day eat lot burger wing lot salty flavorful food flavor additives message n fuck w brain chemistry never ate green grow day eat salad fruit healthy fat add tblspn olive oil mixed help tremendously mood felt much good use angry time also gluck crazy drink shake day make blender throw bunch salad green along w cut whole apple orange carrot broccoli peanut butter apple cider vinegar hamulayian salt tablespoon olive oil twice day college midterm come week even stress reason hope helpsfolded_handsfolded_handsfolded_hands</t>
+          <t>change diet help within day eat lot burger wing lot salty flavorful food flavor additives message n fuck w brain chemistry never ate green grow day eat salad fruit healthy fat add tblspn olive oil mixed help tremendously mood felt much good use angry time also gluck crazy drink shake day make blender throw bunch salad green along w cut whole apple orange carrot broccoli peanut butter apple cider vinegar hamulayian salt tablespoon olive oil twice day college midterm come week even stress reason hope help</t>
         </is>
       </c>
       <c r="C758" t="inlineStr">
@@ -14157,7 +14157,7 @@
       </c>
       <c r="B809" t="inlineStr">
         <is>
-          <t>hahahacrying_face sad even suicidal know must die see get back wow life wish disease snatch away something might regret</t>
+          <t>hahaha sad even suicidal know must die see get back wow life wish disease snatch away something might regret</t>
         </is>
       </c>
       <c r="C809" t="inlineStr">
@@ -15785,7 +15785,7 @@
       </c>
       <c r="B905" t="inlineStr">
         <is>
-          <t>meantime think plant flower hang friend also try make comic way suggest get help already go therapist take ad can not handle life anymore school hard constantly feel tired mark get bad lose motivation keep go reason feel like share know maybe couple month feel well thanks advance sparkling_heart</t>
+          <t>meantime think plant flower hang friend also try make comic way suggest get help already go therapist take ad can not handle life anymore school hard constantly feel tired mark get bad lose motivation keep go reason feel like share know maybe couple month feel well thanks advance</t>
         </is>
       </c>
       <c r="C905" t="inlineStr">
@@ -15989,7 +15989,7 @@
       </c>
       <c r="B917" t="inlineStr">
         <is>
-          <t>care others would feel anymore motivation move forward feel hat feel like anyone love feel like anyone care already hate little friend want people talk know want keep away like nuisance probably mean sooner later go go fuck happy year old girl nothing live forupsidedown_face great</t>
+          <t>care others would feel anymore motivation move forward feel hat feel like anyone love feel like anyone care already hate little friend want people talk know want keep away like nuisance probably mean sooner later go go fuck happy year old girl nothing live great</t>
         </is>
       </c>
       <c r="C917" t="inlineStr">
@@ -16737,7 +16737,7 @@
       </c>
       <c r="B961" t="inlineStr">
         <is>
-          <t>therapist professional anyone need someone talk order get tough time tonight red_heart</t>
+          <t>therapist professional anyone need someone talk order get tough time tonight</t>
         </is>
       </c>
       <c r="C961" t="inlineStr">
@@ -16800,7 +16800,7 @@
     <row r="965">
       <c r="A965" t="inlineStr">
         <is>
-          <t>check_mark_buttonyo check_mark_buttonno school check_mark_button family hat check_mark_button alcooholic</t>
+          <t>yo school family hat alcooholic</t>
         </is>
       </c>
       <c r="B965" t="inlineStr">
@@ -19173,7 +19173,7 @@
       </c>
       <c r="B1105" t="inlineStr">
         <is>
-          <t>thing hold marriage sort together come today family dinner tomorrow nothing argue stupid shit guess tire even fake yesterday birthday party friend course great mainly attempt get dopaminetrade_mark people consider friend live together try shit would bind simple stuff like cook bit common household chore around kitchen common place go drugstore someone sick stuff feedback ask something something like bag cold food know call bag put frozen stuff go grocery store bat eye help find asked someone text get instant ramen store whoop sorry guess forget work treat like everyman almost everyone constantly forgets shit ask rely feel completely alone like alone person rely close one make sick social interaction make sick work make sick constant struggle mental complication make sick corrupted country make sick whole world make sick weird chinese virus literally make people sick consider pussy come suicide already attempt know get impulse third hope would lucky time</t>
+          <t>thing hold marriage sort together come today family dinner tomorrow nothing argue stupid shit guess tire even fake yesterday birthday party friend course great mainly attempt get dopamine people consider friend live together try shit would bind simple stuff like cook bit common household chore around kitchen common place go drugstore someone sick stuff feedback ask something something like bag cold food know call bag put frozen stuff go grocery store bat eye help find asked someone text get instant ramen store whoop sorry guess forget work treat like everyman almost everyone constantly forgets shit ask rely feel completely alone like alone person rely close one make sick social interaction make sick work make sick constant struggle mental complication make sick corrupted country make sick whole world make sick weird chinese virus literally make people sick consider pussy come suicide already attempt know get impulse third hope would lucky time</t>
         </is>
       </c>
       <c r="C1105" t="inlineStr">
@@ -21558,7 +21558,7 @@
       </c>
       <c r="B1246" t="inlineStr">
         <is>
-          <t>clean depression cave today room disgusting start early morning yesterday work day day today still finish till tomorrow take picture shame thishttpsimgurcomajjyd bad bag full trash room get love bad week face_with_rolling_eyes like month though</t>
+          <t>clean depression cave today room disgusting start early morning yesterday work day day today still finish till tomorrow take picture shame thishttpsimgurcomajjyd bad bag full trash room get love bad week like month though</t>
         </is>
       </c>
       <c r="C1246" t="inlineStr">
@@ -22064,7 +22064,7 @@
       </c>
       <c r="B1276" t="inlineStr">
         <is>
-          <t>guess finally grown ball fulfil plan hopefully go well deal thanks put long love victory_hand</t>
+          <t>guess finally grown ball fulfil plan hopefully go well deal thanks put long love</t>
         </is>
       </c>
       <c r="C1276" t="inlineStr">
@@ -22217,7 +22217,7 @@
       </c>
       <c r="B1285" t="inlineStr">
         <is>
-          <t>year shut sometimes social anxiety bad could step house go near window mental health bad could work finish school decide go back school dependent longtime make feel awful element abuse past think fully trust anyone die get high pay job without degree hurt backi terrible back neurological problem leave something like strip suicide point class get intense already behind online class post deadline prioritize class work around hoursweek keep quality highi aim class supposedly grade harshlyso far b something work hour anyway behind online class try make time catch seem impossible person class take much time hour studio homework take maybe hour usually trouble manage time hardly see see stay late play game intimacy month otherwise like xmonth thing help chores unless ask bunch time even though make chore chart u look aton fridge give thing keep promise choresshowerbrush teeth basic thing actually say would chores go back schoollike would do worry worried left thing bit realized correct concern house start look trash talk change topic recite meme kiss maybe twice day otherwise glue phone watch youtube videos quit video game time consume switch video instead addict phone get bus last year passenger usually phone drive nothing drive anxiety work car stress right feel totally alone literally time see therapist even time see doctor checkups work schoolhomeworkand home painfully shy awkward friend join club make friend seem impossible people try befriend seem know interact amazing conversation another top performer class difficult work anticipate become friend try know reciprocate tell make thing uncomfortable react never start form friendship make sense class kid try befriend autism come across pretty brash try remind condition take thing personally sometimes can not help feel terrible time close feel awkward think seem genuinely friendly time mind guess much stress point everything get whole class also pretty distract usually bearable stress wear thing relieve yesterday get grade back quiz friendly note try speak critiquei design student art class make mental note make sure speak critique last night panic first panic want do paint beforehand plan properly always slow everything keep mess finish time seem others finish make feel little good critique come aforementioned kid stand next always uncomfortably close front could see paintings panic increase want rude say anything planned painting critique call order panic disorder cause dissociation stress social anxiety panic mind go blank happen day ago dog unfortunately aggressive dog neighborhood strong dog fortunately point bf experience lunged dog strong enough pull back panickedmind go blank stand mind thing could think like idea feeling alarm could speak move neighbor seem mind give dog treat felt terrible know fix critique mind blank know say absorbed thing others say mind flush tried speak speak thinking time difficult guess stupid usually think long time speak think write know thinkspeak quickly felt like cry could wait pack start draw assignmentuntil realize would forget important supply grow abusive parent dad pretty absent work lot home complete as would constantly provoke old brother harshly pick mom damage somehow grow think good cop taught think could wrong perfect always right upset even seemingly unreasonable mental gymnastics justify example intervene argument dad finance year old understand bad person love mom mom bathroom th time week razor blade would psychiatrist beg come outreason eventually realize say anything eventually still realize could probably leave would come soon anyway around guess talk respond come literally run corner yelled love eat disorder evil dirty slut even though allow house must look something do person mom say guess young child mostly raise grandparent nextdoor would sleep house often would cry sleep every night think mom mad every day would blame something even get blame dad lose even know mom yell back door yard neighborhood kid outside tell would better bring back right friend assume thiefbecause yo can not drive never go anywhere reason money definitely get caught random money point face_with_rolling_eyes point around start self harm understand apparently do upset always apparent major mother pain person love world matter think parent destroy education ongoing argument funsies guess plan graduate gtfo physically bully school point arm near broken every day beg homeschooled plan able focus school without bully graduate early get away family nd grade first year homeschooling skip grade work everything math get maybe grade equivalent current grade public school work parent would argue public homeschooling switch back forth least school semester would public school august month homeschooled obviously ruin extra work would do become discouraged th grade begin lot trouble math mom refuse help say learn disability could learn itand help lovely psychotic step sister instead would public school would often go humiliated explain could finish homework point allow outsidemy grandparent move due stress embrace reclusive tell wanted way whenever people would think odd mom would huff back could speak say everyone friend look back remember dad tell mom coddle much kept people want time think ridiculous see right need soothe blame everything misery get old decide wanted try social would say yes every single opportunity every terrible idea end abused predatory opportunist turn caused major anxiety ever become reclusive ever hold stable job friend since time year ago abusive thing great year move year ago year thing pretty good far go obviously time feel effort person feel shitty couple year ago find terrible situation decide option prostitution strip drug suicide mass apply job would receive response never qualify anything retail bad experience pay enough stop eat become alcoholic little fund attempt suicide somewhere near time week average month straight almost succeed bf unexpectedly come home early send hospital thing get well get threw away antidepressant since feeling felt inappropriate relation thought situation resume weekly attempt otherwise would lie bed try get fear killing suck last year get little well end year decide go back school decide rather abruptly time seek diagnosis learn disability think obviously diagnosis anxiety disorder recurrent major depressive disorder assume would receive accommodation do instead tried plow feeling intentionally make uncomfortable joining club go campus person adjust quickly would hop real world talk social skill care real world old already expose many job field attempt aware feel like failure overload want back know deal everything get help nothing outside school work home need good balance literally way make happen club meet week paper x month new club show become club leader force social situation hope head tell try talk garbage come old everyone else awkward suppose immature stupid social standard feel like go make straight feel like deserve art never look good even spending hour work need make work know know change year instant desperately want want different want anymore meantime try squeeze time get little sleep time room even interact talk anything feel really void affection social interaction right well anything fun use walk every day something lessen frequency nerve pain even time weather shit anyway find gaming fun like sit exhaust even know get anymore frustrated life everything dulli stressedlonely honestly hate everything awful really hate become really sick first week school bronchitis week get well feel like happen really fuck lot since energy know manage everything socialize feel like kill know even properly way totally awful look get away pain last minute life could least peaceful would well ideal really wish assist suicide chronically suicidal people thing sometimes</t>
+          <t>year shut sometimes social anxiety bad could step house go near window mental health bad could work finish school decide go back school dependent longtime make feel awful element abuse past think fully trust anyone die get high pay job without degree hurt backi terrible back neurological problem leave something like strip suicide point class get intense already behind online class post deadline prioritize class work around hoursweek keep quality highi aim class supposedly grade harshlyso far b something work hour anyway behind online class try make time catch seem impossible person class take much time hour studio homework take maybe hour usually trouble manage time hardly see see stay late play game intimacy month otherwise like xmonth thing help chores unless ask bunch time even though make chore chart u look aton fridge give thing keep promise choresshowerbrush teeth basic thing actually say would chores go back schoollike would do worry worried left thing bit realized correct concern house start look trash talk change topic recite meme kiss maybe twice day otherwise glue phone watch youtube videos quit video game time consume switch video instead addict phone get bus last year passenger usually phone drive nothing drive anxiety work car stress right feel totally alone literally time see therapist even time see doctor checkups work schoolhomeworkand home painfully shy awkward friend join club make friend seem impossible people try befriend seem know interact amazing conversation another top performer class difficult work anticipate become friend try know reciprocate tell make thing uncomfortable react never start form friendship make sense class kid try befriend autism come across pretty brash try remind condition take thing personally sometimes can not help feel terrible time close feel awkward think seem genuinely friendly time mind guess much stress point everything get whole class also pretty distract usually bearable stress wear thing relieve yesterday get grade back quiz friendly note try speak critiquei design student art class make mental note make sure speak critique last night panic first panic want do paint beforehand plan properly always slow everything keep mess finish time seem others finish make feel little good critique come aforementioned kid stand next always uncomfortably close front could see paintings panic increase want rude say anything planned painting critique call order panic disorder cause dissociation stress social anxiety panic mind go blank happen day ago dog unfortunately aggressive dog neighborhood strong dog fortunately point bf experience lunged dog strong enough pull back panickedmind go blank stand mind thing could think like idea feeling alarm could speak move neighbor seem mind give dog treat felt terrible know fix critique mind blank know say absorbed thing others say mind flush tried speak speak thinking time difficult guess stupid usually think long time speak think write know thinkspeak quickly felt like cry could wait pack start draw assignmentuntil realize would forget important supply grow abusive parent dad pretty absent work lot home complete as would constantly provoke old brother harshly pick mom damage somehow grow think good cop taught think could wrong perfect always right upset even seemingly unreasonable mental gymnastics justify example intervene argument dad finance year old understand bad person love mom mom bathroom th time week razor blade would psychiatrist beg come outreason eventually realize say anything eventually still realize could probably leave would come soon anyway around guess talk respond come literally run corner yelled love eat disorder evil dirty slut even though allow house must look something do person mom say guess young child mostly raise grandparent nextdoor would sleep house often would cry sleep every night think mom mad every day would blame something even get blame dad lose even know mom yell back door yard neighborhood kid outside tell would better bring back right friend assume thiefbecause yo can not drive never go anywhere reason money definitely get caught random money point point around start self harm understand apparently do upset always apparent major mother pain person love world matter think parent destroy education ongoing argument funsies guess plan graduate gtfo physically bully school point arm near broken every day beg homeschooled plan able focus school without bully graduate early get away family nd grade first year homeschooling skip grade work everything math get maybe grade equivalent current grade public school work parent would argue public homeschooling switch back forth least school semester would public school august month homeschooled obviously ruin extra work would do become discouraged th grade begin lot trouble math mom refuse help say learn disability could learn itand help lovely psychotic step sister instead would public school would often go humiliated explain could finish homework point allow outsidemy grandparent move due stress embrace reclusive tell wanted way whenever people would think odd mom would huff back could speak say everyone friend look back remember dad tell mom coddle much kept people want time think ridiculous see right need soothe blame everything misery get old decide wanted try social would say yes every single opportunity every terrible idea end abused predatory opportunist turn caused major anxiety ever become reclusive ever hold stable job friend since time year ago abusive thing great year move year ago year thing pretty good far go obviously time feel effort person feel shitty couple year ago find terrible situation decide option prostitution strip drug suicide mass apply job would receive response never qualify anything retail bad experience pay enough stop eat become alcoholic little fund attempt suicide somewhere near time week average month straight almost succeed bf unexpectedly come home early send hospital thing get well get threw away antidepressant since feeling felt inappropriate relation thought situation resume weekly attempt otherwise would lie bed try get fear killing suck last year get little well end year decide go back school decide rather abruptly time seek diagnosis learn disability think obviously diagnosis anxiety disorder recurrent major depressive disorder assume would receive accommodation do instead tried plow feeling intentionally make uncomfortable joining club go campus person adjust quickly would hop real world talk social skill care real world old already expose many job field attempt aware feel like failure overload want back know deal everything get help nothing outside school work home need good balance literally way make happen club meet week paper x month new club show become club leader force social situation hope head tell try talk garbage come old everyone else awkward suppose immature stupid social standard feel like go make straight feel like deserve art never look good even spending hour work need make work know know change year instant desperately want want different want anymore meantime try squeeze time get little sleep time room even interact talk anything feel really void affection social interaction right well anything fun use walk every day something lessen frequency nerve pain even time weather shit anyway find gaming fun like sit exhaust even know get anymore frustrated life everything dulli stressedlonely honestly hate everything awful really hate become really sick first week school bronchitis week get well feel like happen really fuck lot since energy know manage everything socialize feel like kill know even properly way totally awful look get away pain last minute life could least peaceful would well ideal really wish assist suicide chronically suicidal people thing sometimes</t>
         </is>
       </c>
       <c r="C1285" t="inlineStr">
@@ -22808,7 +22808,7 @@
       </c>
       <c r="B1320" t="inlineStr">
         <is>
-          <t>lose know anymore can not control emotion anymore piss second cry next laughing want end second later try trick help nothing depressed lately everything happen life work personal legal always feel alone seriously want end lately want go anymore damn hard sick tire living life full torture pensive_face</t>
+          <t>lose know anymore can not control emotion anymore piss second cry next laughing want end second later try trick help nothing depressed lately everything happen life work personal legal always feel alone seriously want end lately want go anymore damn hard sick tire living life full torture</t>
         </is>
       </c>
       <c r="C1320" t="inlineStr">
@@ -24768,7 +24768,7 @@
       </c>
       <c r="B1436" t="inlineStr">
         <is>
-          <t>meet girl month ago feel love quick portugal slovenia think long distance feel like go work talk day ago tell can not friends make suffer seem problem can not get watch somebody drift away wait hurt much thing say amazing bad want stay can not fall depression tell go stay know capable hurt year think get crawls back fast ahhhhh feel like egoistical needy piece shit can not get fact fuck shit fuck life thanks listen red_heart</t>
+          <t>meet girl month ago feel love quick portugal slovenia think long distance feel like go work talk day ago tell can not friends make suffer seem problem can not get watch somebody drift away wait hurt much thing say amazing bad want stay can not fall depression tell go stay know capable hurt year think get crawls back fast ahhhhh feel like egoistical needy piece shit can not get fact fuck shit fuck life thanks listen</t>
         </is>
       </c>
       <c r="C1436" t="inlineStr">
@@ -25256,12 +25256,12 @@
     <row r="1465">
       <c r="A1465" t="inlineStr">
         <is>
-          <t>vicious circle lonelinessdepression counterclockwise_arrows_button</t>
+          <t>vicious circle lonelinessdepression</t>
         </is>
       </c>
       <c r="B1465" t="inlineStr">
         <is>
-          <t>alone lack self confidence left_arrow_curving_right able give receive love affection left_arrow_curving_right feel unwantedundesired left_arrow_curving_right loss self confidence intensifies left_arrow_curving_right isolation opportunity meet new people left_arrow_curving_right depression left_arrow_curving_right feel worthless left_arrow_curving_right achieve anything ashamed repeat_single_button</t>
+          <t>alone lack self confidence able give receive love affection feeling unwantedundesired loss self confidence intensifies isolation opportunity meet new people depression feel worthless achieve anything ashamed</t>
         </is>
       </c>
       <c r="C1465" t="inlineStr">
@@ -25409,12 +25409,12 @@
     <row r="1474">
       <c r="A1474" t="inlineStr">
         <is>
-          <t>go slit wrist clown_faceclown_face</t>
+          <t>go slit wrist</t>
         </is>
       </c>
       <c r="B1474" t="inlineStr">
         <is>
-          <t>fuck asshole clown_faceglobe_showing_EuropeAfricaglobe_showing_EuropeAfricaglobe_showing_EuropeAfricaglobe_showing_EuropeAfricamiddle_fingermiddle_fingermiddle_fingermiddle_fingermiddle_finger</t>
+          <t>fuck asshole</t>
         </is>
       </c>
       <c r="C1474" t="inlineStr">

</xml_diff>